<commit_message>
Changes: new DB from mobile phone; new algorithm for extracting currency; calculated quality level for different detectors and descriptors and matchrs with different DBs
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>SIFT</t>
   </si>
@@ -85,6 +85,36 @@
   </si>
   <si>
     <t>14% 7m BF</t>
+  </si>
+  <si>
+    <t>Partial wiki DB</t>
+  </si>
+  <si>
+    <t>Full wiki DB</t>
+  </si>
+  <si>
+    <t>Partial phone DB</t>
+  </si>
+  <si>
+    <t>23% 35m</t>
+  </si>
+  <si>
+    <t>27% 21m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23% 32m </t>
+  </si>
+  <si>
+    <t>Phone full DB</t>
+  </si>
+  <si>
+    <t>With preprocessing</t>
+  </si>
+  <si>
+    <t>With preprocessing images with one currency</t>
+  </si>
+  <si>
+    <t>33% 11m</t>
   </si>
 </sst>
 </file>
@@ -120,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -402,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,6 +444,7 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
@@ -511,6 +543,64 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>